<commit_message>
[LC-260] Improve the validator of JSON and Excel files (3)
Signed-off-by: OUESLATI Wyem Ext <wyem.oueslati@rte-france.com>
</commit_message>
<xml_diff>
--- a/message_models/xlsx/ProcessFailed_SampleData_v4.xlsx
+++ b/message_models/xlsx/ProcessFailed_SampleData_v4.xlsx
@@ -454,7 +454,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="20">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -526,6 +526,48 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
@@ -579,7 +621,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="53">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -680,19 +722,23 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -700,11 +746,35 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -720,7 +790,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -728,39 +798,39 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="8" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="8" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -850,7 +920,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+      <selection pane="bottomLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -860,19 +930,20 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="32.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="25.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="57.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="21.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="19.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="16.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="14.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="1" width="19.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="1" width="19.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="24.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="19.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="13.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="25.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1008" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1007" min="19" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1008" style="0" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1022,15 +1093,15 @@
       <c r="A6" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="26" t="s">
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="25" t="s">
         <v>31</v>
       </c>
       <c r="I6" s="16"/>
@@ -1049,15 +1120,15 @@
       <c r="A7" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="26" t="s">
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="25" t="s">
         <v>33</v>
       </c>
       <c r="I7" s="16"/>
@@ -1073,24 +1144,24 @@
       <c r="S7" s="23"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21" t="s">
+      <c r="C8" s="27"/>
+      <c r="D8" s="27" t="s">
         <v>36</v>
       </c>
       <c r="E8" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21" t="s">
+      <c r="F8" s="27"/>
+      <c r="G8" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="H8" s="22" t="n">
+      <c r="H8" s="29" t="n">
         <v>0</v>
       </c>
       <c r="I8" s="16"/>
@@ -1100,28 +1171,30 @@
       <c r="M8" s="16"/>
       <c r="N8" s="16"/>
       <c r="O8" s="16"/>
-      <c r="P8" s="29"/>
+      <c r="P8" s="30"/>
       <c r="Q8" s="16"/>
       <c r="R8" s="16"/>
       <c r="S8" s="23"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="C9" s="33"/>
+      <c r="D9" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="G9" s="30" t="s">
+      <c r="F9" s="35"/>
+      <c r="G9" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="H9" s="22" t="n">
+      <c r="H9" s="37" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1151,149 +1224,152 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="38" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="D2" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="33" t="s">
+      <c r="G2" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="H2" s="33" t="s">
+      <c r="H2" s="40" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="E3" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="F3" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="33" t="s">
+      <c r="G3" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="H3" s="33" t="s">
+      <c r="H3" s="40" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="E4" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="F4" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="G4" s="33" t="s">
+      <c r="G4" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="H4" s="33" t="s">
+      <c r="H4" s="40" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="33" t="s">
+      <c r="D5" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="33" t="s">
+      <c r="E5" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="33" t="s">
+      <c r="F5" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="G5" s="33" t="s">
+      <c r="G5" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="33" t="s">
+      <c r="H5" s="40" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E6" s="34"/>
-      <c r="G6" s="34"/>
+      <c r="E6" s="41"/>
+      <c r="G6" s="41"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E7" s="34"/>
-      <c r="G7" s="34"/>
+      <c r="E7" s="41"/>
+      <c r="G7" s="41"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E8" s="34"/>
-      <c r="G8" s="34"/>
+      <c r="E8" s="41"/>
+      <c r="G8" s="41"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1323,406 +1399,406 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="12.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="6.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="9.13"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="36" t="s">
+      <c r="E3" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="G3" s="36" t="s">
+      <c r="G3" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="H3" s="36" t="s">
+      <c r="H3" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="I3" s="36" t="s">
+      <c r="I3" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="J3" s="36" t="s">
+      <c r="J3" s="43" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="35" t="n">
+      <c r="B4" s="42" t="n">
         <v>1</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="37" t="s">
+      <c r="E4" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="F4" s="35" t="s">
+      <c r="F4" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="G4" s="38" t="s">
+      <c r="G4" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="H4" s="39"/>
-      <c r="I4" s="38" t="s">
+      <c r="H4" s="46"/>
+      <c r="I4" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="J4" s="39"/>
+      <c r="J4" s="46"/>
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="40" t="s">
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="H5" s="41"/>
-      <c r="I5" s="40" t="s">
+      <c r="H5" s="48"/>
+      <c r="I5" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="J5" s="41"/>
+      <c r="J5" s="48"/>
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="42" t="s">
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="E6" s="42" t="s">
+      <c r="E6" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="F6" s="35" t="s">
+      <c r="F6" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="G6" s="40" t="s">
+      <c r="G6" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="H6" s="41"/>
-      <c r="I6" s="40" t="s">
+      <c r="H6" s="48"/>
+      <c r="I6" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="J6" s="41"/>
+      <c r="J6" s="48"/>
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="35"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="40" t="s">
+      <c r="B7" s="42"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="H7" s="41"/>
-      <c r="I7" s="40" t="s">
+      <c r="H7" s="48"/>
+      <c r="I7" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="J7" s="41"/>
+      <c r="J7" s="48"/>
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="35"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="43" t="s">
+      <c r="B8" s="42"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="E8" s="43" t="s">
+      <c r="E8" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="F8" s="35" t="s">
+      <c r="F8" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="G8" s="40" t="s">
+      <c r="G8" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="H8" s="41"/>
-      <c r="I8" s="40" t="s">
+      <c r="H8" s="48"/>
+      <c r="I8" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="J8" s="41"/>
+      <c r="J8" s="48"/>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="35"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="40" t="s">
+      <c r="B9" s="42"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="I9" s="41"/>
-      <c r="J9" s="40" t="s">
+      <c r="I9" s="48"/>
+      <c r="J9" s="47" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="44" t="s">
+      <c r="B10" s="42"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="E10" s="44" t="s">
+      <c r="E10" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="F10" s="35" t="s">
+      <c r="F10" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="G10" s="41"/>
-      <c r="H10" s="40" t="s">
+      <c r="G10" s="48"/>
+      <c r="H10" s="47" t="s">
         <v>78</v>
       </c>
-      <c r="I10" s="41"/>
-      <c r="J10" s="40" t="s">
+      <c r="I10" s="48"/>
+      <c r="J10" s="47" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="35"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="40" t="s">
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="48"/>
+      <c r="H11" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="I11" s="41"/>
-      <c r="J11" s="40" t="s">
+      <c r="I11" s="48"/>
+      <c r="J11" s="47" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="35"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="45" t="s">
+      <c r="B12" s="42"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="52" t="s">
         <v>82</v>
       </c>
-      <c r="E12" s="45" t="s">
+      <c r="E12" s="52" t="s">
         <v>83</v>
       </c>
-      <c r="F12" s="35" t="s">
+      <c r="F12" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="G12" s="41"/>
-      <c r="H12" s="40" t="s">
+      <c r="G12" s="48"/>
+      <c r="H12" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="I12" s="41"/>
-      <c r="J12" s="40" t="s">
+      <c r="I12" s="48"/>
+      <c r="J12" s="47" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="40" t="s">
+      <c r="B13" s="42"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="48"/>
+      <c r="H13" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="I13" s="41"/>
-      <c r="J13" s="40" t="s">
+      <c r="I13" s="48"/>
+      <c r="J13" s="47" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="35"/>
-      <c r="C14" s="35" t="s">
+      <c r="B14" s="42"/>
+      <c r="C14" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="D14" s="37" t="s">
+      <c r="D14" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="E14" s="37" t="s">
+      <c r="E14" s="44" t="s">
         <v>91</v>
       </c>
-      <c r="F14" s="35" t="s">
+      <c r="F14" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="G14" s="40" t="s">
+      <c r="G14" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="H14" s="41"/>
-      <c r="I14" s="40" t="s">
+      <c r="H14" s="48"/>
+      <c r="I14" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="J14" s="41"/>
+      <c r="J14" s="48"/>
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="40" t="s">
+      <c r="B15" s="42"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="H15" s="41"/>
-      <c r="I15" s="40" t="s">
+      <c r="H15" s="48"/>
+      <c r="I15" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="J15" s="41"/>
+      <c r="J15" s="48"/>
     </row>
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="35"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="42" t="s">
+      <c r="B16" s="42"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="E16" s="42" t="s">
+      <c r="E16" s="49" t="s">
         <v>93</v>
       </c>
-      <c r="F16" s="35" t="s">
+      <c r="F16" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="G16" s="40" t="s">
+      <c r="G16" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="H16" s="41"/>
-      <c r="I16" s="40" t="s">
+      <c r="H16" s="48"/>
+      <c r="I16" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="J16" s="41"/>
+      <c r="J16" s="48"/>
     </row>
     <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="35"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="40" t="s">
+      <c r="B17" s="42"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="H17" s="41"/>
-      <c r="I17" s="40" t="s">
+      <c r="H17" s="48"/>
+      <c r="I17" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="J17" s="41"/>
+      <c r="J17" s="48"/>
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="35"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="43" t="s">
+      <c r="B18" s="42"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="E18" s="43" t="s">
+      <c r="E18" s="50" t="s">
         <v>95</v>
       </c>
-      <c r="F18" s="35" t="s">
+      <c r="F18" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="G18" s="40" t="s">
+      <c r="G18" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="H18" s="41"/>
-      <c r="I18" s="40" t="s">
+      <c r="H18" s="48"/>
+      <c r="I18" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="J18" s="41"/>
+      <c r="J18" s="48"/>
     </row>
     <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="35"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="43"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="41"/>
-      <c r="H19" s="40" t="s">
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="I19" s="41"/>
-      <c r="J19" s="40" t="s">
+      <c r="I19" s="48"/>
+      <c r="J19" s="47" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="35"/>
-      <c r="C20" s="35"/>
-      <c r="D20" s="44" t="s">
+      <c r="B20" s="42"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="51" t="s">
         <v>96</v>
       </c>
-      <c r="E20" s="44" t="s">
+      <c r="E20" s="51" t="s">
         <v>97</v>
       </c>
-      <c r="F20" s="35" t="s">
+      <c r="F20" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="G20" s="41"/>
-      <c r="H20" s="40" t="s">
+      <c r="G20" s="48"/>
+      <c r="H20" s="47" t="s">
         <v>78</v>
       </c>
-      <c r="I20" s="41"/>
-      <c r="J20" s="40" t="s">
+      <c r="I20" s="48"/>
+      <c r="J20" s="47" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="35"/>
-      <c r="C21" s="35"/>
-      <c r="D21" s="44"/>
-      <c r="E21" s="44"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="41"/>
-      <c r="H21" s="40" t="s">
+      <c r="B21" s="42"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="51"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="48"/>
+      <c r="H21" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="I21" s="41"/>
-      <c r="J21" s="40" t="s">
+      <c r="I21" s="48"/>
+      <c r="J21" s="47" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="35"/>
-      <c r="C22" s="35"/>
-      <c r="D22" s="45" t="s">
+      <c r="B22" s="42"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="52" t="s">
         <v>98</v>
       </c>
-      <c r="E22" s="45" t="s">
+      <c r="E22" s="52" t="s">
         <v>99</v>
       </c>
-      <c r="F22" s="35" t="s">
+      <c r="F22" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="G22" s="41"/>
-      <c r="H22" s="40" t="s">
+      <c r="G22" s="48"/>
+      <c r="H22" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="I22" s="41"/>
-      <c r="J22" s="40" t="s">
+      <c r="I22" s="48"/>
+      <c r="J22" s="47" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="35"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="41"/>
-      <c r="H23" s="40" t="s">
+      <c r="B23" s="42"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="I23" s="41"/>
-      <c r="J23" s="40" t="s">
+      <c r="I23" s="48"/>
+      <c r="J23" s="47" t="s">
         <v>88</v>
       </c>
     </row>

</xml_diff>